<commit_message>
All utilMethods are now non-static
</commit_message>
<xml_diff>
--- a/Data/userData.xlsx
+++ b/Data/userData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\smplfw\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Mac2Data/AutomationUIFramework/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3601D4-B22C-0D45-98BB-6B687018F752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -24,28 +25,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>uname</t>
-  </si>
-  <si>
-    <t>pwd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>currentAddress</t>
+  </si>
+  <si>
+    <t>permanentAdd</t>
+  </si>
+  <si>
+    <t>Davinder Sharma</t>
+  </si>
+  <si>
+    <t>dav@gmail.com</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>patna</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>rohit@gmail.cm</t>
+  </si>
+  <si>
+    <t>marathali</t>
+  </si>
+  <si>
+    <t>belgam</t>
+  </si>
+  <si>
+    <t>Thushar</t>
+  </si>
+  <si>
+    <t>thushar@gmail.com</t>
+  </si>
+  <si>
+    <t>multiplex</t>
+  </si>
+  <si>
+    <t>coorg</t>
+  </si>
+  <si>
+    <t>Soumik</t>
+  </si>
+  <si>
+    <t>soumik@gmail.com</t>
+  </si>
+  <si>
+    <t>vkrPG</t>
+  </si>
+  <si>
+    <t>aasam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,17 +125,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,40 +416,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="J2" s="2"/>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6BE490B6-E774-7F42-A1CA-36CACF235379}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{51AD86B1-282E-0442-84C5-1D67863720B7}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{DE11F749-497D-3F4F-8EE2-5798C0C2BD9D}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{2202A477-A340-EF4D-8EBE-F7BB25CC9BD3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>